<commit_message>
risultati F27 e F79 precond, da salvare risultati convergenza 27
</commit_message>
<xml_diff>
--- a/F27_truncated/results_f27_3_quad.xlsx
+++ b/F27_truncated/results_f27_3_quad.xlsx
@@ -245,13 +245,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="0">
-        <v>0.0091987454545454529</v>
+        <v>0.0078786363636363654</v>
       </c>
       <c r="C2" s="0">
-        <v>0.16989164545454546</v>
+        <v>0.1122847090909091</v>
       </c>
       <c r="D2" s="0">
-        <v>0.92635266363636359</v>
+        <v>0.74987999090909097</v>
       </c>
     </row>
     <row r="3">
@@ -336,22 +336,22 @@
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0">
-        <v>0.0050886727272727271</v>
+        <v>0.0030769909090909088</v>
       </c>
       <c r="D2" s="0">
-        <v>0.0041682454545454543</v>
+        <v>0.0026921727272727269</v>
       </c>
       <c r="E2" s="0">
-        <v>0.0042735363636363637</v>
+        <v>0.0025968181818181815</v>
       </c>
       <c r="F2" s="0">
-        <v>0.0058474727272727267</v>
+        <v>0.002705063636363636</v>
       </c>
       <c r="G2" s="0">
-        <v>0.0040470454545454551</v>
+        <v>0.0029010363636363637</v>
       </c>
       <c r="H2" s="0">
-        <v>0.0091987454545454529</v>
+        <v>0.0078786363636363654</v>
       </c>
     </row>
     <row r="3">
@@ -359,25 +359,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>0.021471000000000001</v>
+        <v>0.0053664999999999997</v>
       </c>
       <c r="C3" s="0">
-        <v>0.0055300363636363635</v>
+        <v>0.0034495545454545458</v>
       </c>
       <c r="D3" s="0">
-        <v>0.0053411090909090903</v>
+        <v>0.003366909090909091</v>
       </c>
       <c r="E3" s="0">
-        <v>0.0046718181818181815</v>
+        <v>0.0030955909090909089</v>
       </c>
       <c r="F3" s="0">
-        <v>0.0056509000000000012</v>
+        <v>0.0036196999999999996</v>
       </c>
       <c r="G3" s="0">
-        <v>0.0051885909090909083</v>
+        <v>0.0035483636363636368</v>
       </c>
       <c r="H3" s="0">
-        <v>0.0091987454545454529</v>
+        <v>0.0078786363636363654</v>
       </c>
     </row>
   </sheetData>
@@ -590,10 +590,10 @@
   <cols>
     <col min="1" max="1" width="4.6640625" customWidth="true"/>
     <col min="2" max="2" width="6.6640625" customWidth="true"/>
-    <col min="3" max="3" width="9.5546875" customWidth="true"/>
+    <col min="3" max="3" width="12.5546875" customWidth="true"/>
     <col min="4" max="4" width="12.5546875" customWidth="true"/>
     <col min="5" max="5" width="12.5546875" customWidth="true"/>
-    <col min="6" max="6" width="12.5546875" customWidth="true"/>
+    <col min="6" max="6" width="9.5546875" customWidth="true"/>
     <col min="7" max="7" width="12.5546875" customWidth="true"/>
     <col min="8" max="8" width="12.5546875" customWidth="true"/>
   </cols>
@@ -630,22 +630,22 @@
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0">
-        <v>0.25721660000000002</v>
+        <v>0.13881184545454542</v>
       </c>
       <c r="D2" s="0">
-        <v>0.22134188181818182</v>
+        <v>0.12278751818181816</v>
       </c>
       <c r="E2" s="0">
-        <v>0.21399624545454543</v>
+        <v>0.12172322727272727</v>
       </c>
       <c r="F2" s="0">
-        <v>0.22167227272727275</v>
+        <v>0.12465450000000002</v>
       </c>
       <c r="G2" s="0">
-        <v>0.21304097272727274</v>
+        <v>0.12769941818181818</v>
       </c>
       <c r="H2" s="0">
-        <v>0.16989164545454546</v>
+        <v>0.1122847090909091</v>
       </c>
     </row>
     <row r="3">
@@ -654,22 +654,22 @@
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="0">
-        <v>0.31234187272727276</v>
+        <v>0.15964258181818181</v>
       </c>
       <c r="D3" s="0">
-        <v>0.29323405454545454</v>
+        <v>0.1527717909090909</v>
       </c>
       <c r="E3" s="0">
-        <v>0.28410462727272728</v>
+        <v>0.17095881818181821</v>
       </c>
       <c r="F3" s="0">
-        <v>0.28064722727272728</v>
+        <v>0.16564358181818181</v>
       </c>
       <c r="G3" s="0">
-        <v>0.27847917272727274</v>
+        <v>0.16776949999999996</v>
       </c>
       <c r="H3" s="0">
-        <v>0.16989164545454546</v>
+        <v>0.1122847090909091</v>
       </c>
     </row>
   </sheetData>
@@ -880,9 +880,9 @@
     <col min="2" max="2" width="6.6640625" customWidth="true"/>
     <col min="3" max="3" width="11.5546875" customWidth="true"/>
     <col min="4" max="4" width="11.5546875" customWidth="true"/>
-    <col min="5" max="5" width="11.5546875" customWidth="true"/>
-    <col min="6" max="6" width="11.5546875" customWidth="true"/>
-    <col min="7" max="7" width="11.5546875" customWidth="true"/>
+    <col min="5" max="5" width="12.5546875" customWidth="true"/>
+    <col min="6" max="6" width="12.5546875" customWidth="true"/>
+    <col min="7" max="7" width="12.5546875" customWidth="true"/>
     <col min="8" max="8" width="12.5546875" customWidth="true"/>
   </cols>
   <sheetData>
@@ -918,22 +918,22 @@
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0">
-        <v>1.3552043363636366</v>
+        <v>1.1326043818181819</v>
       </c>
       <c r="D2" s="0">
-        <v>1.2246344454545457</v>
+        <v>1.0135755363636365</v>
       </c>
       <c r="E2" s="0">
-        <v>1.1511259909090912</v>
+        <v>0.94775871818181823</v>
       </c>
       <c r="F2" s="0">
-        <v>1.1179162181818183</v>
+        <v>0.92712419090909082</v>
       </c>
       <c r="G2" s="0">
-        <v>1.1246843272727274</v>
+        <v>0.89861612727272722</v>
       </c>
       <c r="H2" s="0">
-        <v>0.92635266363636359</v>
+        <v>0.74987999090909097</v>
       </c>
     </row>
     <row r="3">
@@ -941,25 +941,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>2.3830743181818184</v>
+        <v>1.7427456545454545</v>
       </c>
       <c r="C3" s="0">
-        <v>1.6582351818181815</v>
+        <v>1.4515882818181818</v>
       </c>
       <c r="D3" s="0">
-        <v>1.4661527363636362</v>
+        <v>1.2067522181818182</v>
       </c>
       <c r="E3" s="0">
-        <v>1.4226192636363637</v>
+        <v>1.1787489272727274</v>
       </c>
       <c r="F3" s="0">
-        <v>1.4759070999999999</v>
+        <v>1.1249758545454542</v>
       </c>
       <c r="G3" s="0">
-        <v>1.4759894909090912</v>
+        <v>1.148898018181818</v>
       </c>
       <c r="H3" s="0">
-        <v>0.92635266363636359</v>
+        <v>0.74987999090909097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>